<commit_message>
not sure what changed on this here second commit
</commit_message>
<xml_diff>
--- a/thermo_tables.xlsx
+++ b/thermo_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="table 3" sheetId="2" r:id="rId1"/>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1119,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
saving before the long weekend
</commit_message>
<xml_diff>
--- a/thermo_tables.xlsx
+++ b/thermo_tables.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7065" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7065"/>
   </bookViews>
   <sheets>
-    <sheet name="table 3" sheetId="2" r:id="rId1"/>
-    <sheet name="table 4" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="table 3" sheetId="2" r:id="rId2"/>
+    <sheet name="table 4" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>Cations</t>
   </si>
@@ -536,6 +536,527 @@
   </si>
   <si>
     <t>Ions</t>
+  </si>
+  <si>
+    <r>
+      <t>KAl</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Si</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al)O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OH)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>K+</t>
+  </si>
+  <si>
+    <t>Al+++</t>
+  </si>
+  <si>
+    <t>H+</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>oxide</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>n*x</t>
+  </si>
+  <si>
+    <t>n_i</t>
+  </si>
+  <si>
+    <t>n_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_o </t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>ns_intra</t>
+  </si>
+  <si>
+    <t>ns_inter</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <r>
+      <t>ΔH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>xi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(c)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Zi+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(aq)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,Ox</t>
+    </r>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <r>
+      <t>k*(z/2)*ΔH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>xi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(c)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ʃ</t>
+  </si>
+  <si>
+    <r>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>site (first term)</t>
+    </r>
+  </si>
+  <si>
+    <t>k_i</t>
+  </si>
+  <si>
+    <t>Al_o</t>
+  </si>
+  <si>
+    <t>Si_t</t>
+  </si>
+  <si>
+    <t>Al_t</t>
+  </si>
+  <si>
+    <t>E.N.</t>
+  </si>
+  <si>
+    <t>coeff</t>
+  </si>
+  <si>
+    <t>inner bracket</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>second term</t>
+  </si>
+  <si>
+    <t>first term</t>
+  </si>
+  <si>
+    <r>
+      <t>ΔH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>o</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -911,10 +1432,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>(D2*(D2-1)+F2*(F2-1)+G2*(G2-1))/2</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>D2*F2+F2*G2+G2</f>
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>H2+I2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f>D5/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <f>G5*F5</f>
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <f>H5/$C$2</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J5">
+        <f>'table 3'!B3</f>
+        <v>-363.17</v>
+      </c>
+      <c r="K5">
+        <f>'table 3'!C13</f>
+        <v>141</v>
+      </c>
+      <c r="N5">
+        <f>E5*J5</f>
+        <v>-181.58500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f>D6/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H9" si="0">G6*F6</f>
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I9" si="1">H6/$C$2</f>
+        <v>0.25</v>
+      </c>
+      <c r="J6">
+        <f>'table 3'!B8</f>
+        <v>-1675.7</v>
+      </c>
+      <c r="K6">
+        <f>'table 4'!B10</f>
+        <v>-199.63</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N9" si="2">E6*J6</f>
+        <v>-1675.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>D7/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="J7">
+        <f>'table 3'!B8</f>
+        <v>-1675.7</v>
+      </c>
+      <c r="K7">
+        <f>'table 4'!B15</f>
+        <v>-199.63</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>-837.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f>D8/2</f>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <f>'table 3'!B9</f>
+        <v>-910.7</v>
+      </c>
+      <c r="K8">
+        <f>'table 4'!B14</f>
+        <v>-205</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>-2732.1000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J9">
+        <f>'table 4'!B25</f>
+        <v>-249.58</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>-249.58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10">
+        <f>SUM(I5:I9)</f>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>SUM(N5:N9)</f>
+        <v>-5676.8150000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14">
+        <f>ABS('table 4'!C3-'table 4'!C14)</f>
+        <v>738.32999999999993</v>
+      </c>
+      <c r="E14">
+        <f>ABS('table 4'!C3-'table 4'!C15)</f>
+        <v>713.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <f>ABS('table 4'!C10-'table 4'!C14)</f>
+        <v>33.579999999999984</v>
+      </c>
+      <c r="E15">
+        <f>ABS('table 4'!C10-'table 4'!C21)</f>
+        <v>22.699999999999989</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16">
+        <f>ABS('table 4'!C14-'table 4'!C15)</f>
+        <v>24.879999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22">
+        <f>I5*I8</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E22">
+        <f>I5*I8</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23">
+        <f>I6*I8</f>
+        <v>0.125</v>
+      </c>
+      <c r="E23">
+        <f>I6*I7</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <f>I7*I8</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29">
+        <f>B14*B22</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:F29" si="3">C14*C22</f>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>15.381874999999997</v>
+      </c>
+      <c r="E29">
+        <f>E14*E22</f>
+        <v>14.863541666666666</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f>SUM(B29:F29)</f>
+        <v>30.245416666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:F30" si="4">B15*B23</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="4"/>
+        <v>4.197499999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>0.70937499999999964</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G33" si="5">SUM(B30:F30)</f>
+        <v>4.9068749999999977</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ref="B31:F31" si="6">B16*B24</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="6"/>
+        <v>1.5549999999999997</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>1.5549999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:F32" si="7">B17*B25</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="8">B18*B26</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f>SUM(G29:G33)</f>
+        <v>36.707291666666663</v>
+      </c>
+      <c r="H34">
+        <f>-C2*G34</f>
+        <v>-440.48749999999995</v>
+      </c>
+      <c r="I34">
+        <f>N10+H34</f>
+        <v>-6117.3025000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>-301.39</v>
+      </c>
+      <c r="I35">
+        <f>N10+H35</f>
+        <v>-5978.2050000000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,12 +2326,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,16 +2623,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>